<commit_message>
Changed the IP addresses for the Netduino
</commit_message>
<xml_diff>
--- a/docs/SignupSheet.xlsx
+++ b/docs/SignupSheet.xlsx
@@ -67,54 +67,6 @@
     <t>bedroom2</t>
   </si>
   <si>
-    <t>192.168.0.2</t>
-  </si>
-  <si>
-    <t>192.168.0.3</t>
-  </si>
-  <si>
-    <t>192.168.0.4</t>
-  </si>
-  <si>
-    <t>192.168.0.5</t>
-  </si>
-  <si>
-    <t>192.168.0.6</t>
-  </si>
-  <si>
-    <t>192.168.0.7</t>
-  </si>
-  <si>
-    <t>192.168.0.8</t>
-  </si>
-  <si>
-    <t>192.168.0.9</t>
-  </si>
-  <si>
-    <t>192.168.0.10</t>
-  </si>
-  <si>
-    <t>192.168.0.11</t>
-  </si>
-  <si>
-    <t>192.168.0.12</t>
-  </si>
-  <si>
-    <t>192.168.0.13</t>
-  </si>
-  <si>
-    <t>192.168.0.14</t>
-  </si>
-  <si>
-    <t>192.168.0.15</t>
-  </si>
-  <si>
-    <t>192.168.0.16</t>
-  </si>
-  <si>
-    <t>192.168.0.17</t>
-  </si>
-  <si>
     <t>Unique Client ID</t>
   </si>
   <si>
@@ -134,6 +86,54 @@
   </si>
   <si>
     <t>doorbell</t>
+  </si>
+  <si>
+    <t>192.168.1.2</t>
+  </si>
+  <si>
+    <t>192.168.1.3</t>
+  </si>
+  <si>
+    <t>192.168.1.4</t>
+  </si>
+  <si>
+    <t>192.168.1.5</t>
+  </si>
+  <si>
+    <t>192.168.1.6</t>
+  </si>
+  <si>
+    <t>192.168.1.7</t>
+  </si>
+  <si>
+    <t>192.168.1.8</t>
+  </si>
+  <si>
+    <t>192.168.1.9</t>
+  </si>
+  <si>
+    <t>192.168.1.10</t>
+  </si>
+  <si>
+    <t>192.168.1.11</t>
+  </si>
+  <si>
+    <t>192.168.1.12</t>
+  </si>
+  <si>
+    <t>192.168.1.13</t>
+  </si>
+  <si>
+    <t>192.168.1.14</t>
+  </si>
+  <si>
+    <t>192.168.1.15</t>
+  </si>
+  <si>
+    <t>192.168.1.16</t>
+  </si>
+  <si>
+    <t>192.168.1.17</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,7 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -542,7 +542,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>0</v>
@@ -563,13 +563,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -585,13 +585,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -607,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -629,13 +629,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -651,13 +651,13 @@
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -673,13 +673,13 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -695,13 +695,13 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -717,13 +717,13 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -739,13 +739,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -761,13 +761,13 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -783,13 +783,13 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -803,7 +803,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -817,7 +817,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -831,7 +831,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -845,7 +845,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -859,7 +859,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H17" s="1"/>
     </row>

</xml_diff>

<commit_message>
fixed a spelling error
</commit_message>
<xml_diff>
--- a/docs/SignupSheet.xlsx
+++ b/docs/SignupSheet.xlsx
@@ -82,9 +82,6 @@
     <t>alarmpanel</t>
   </si>
   <si>
-    <t>extrernaldoor</t>
-  </si>
-  <si>
     <t>doorbell</t>
   </si>
   <si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>192.168.1.19</t>
+  </si>
+  <si>
+    <t>externaldoor</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E10" sqref="E10:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -582,13 +582,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -604,13 +604,13 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4"/>
     </row>
@@ -632,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="4"/>
     </row>
@@ -654,7 +654,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H5" s="4"/>
     </row>
@@ -676,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -698,7 +698,7 @@
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -720,7 +720,7 @@
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="4"/>
     </row>
@@ -742,7 +742,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="4"/>
     </row>
@@ -758,13 +758,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="4"/>
     </row>
@@ -780,13 +780,13 @@
         <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -802,13 +802,13 @@
         <v>7</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H12" s="4"/>
     </row>
@@ -822,7 +822,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="4"/>
     </row>
@@ -836,7 +836,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="4"/>
     </row>
@@ -850,7 +850,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -864,7 +864,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -878,7 +878,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -892,7 +892,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -906,7 +906,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated to remove the IP Addresses and the MAC addresses since DHCP is being used
</commit_message>
<xml_diff>
--- a/docs/SignupSheet.xlsx
+++ b/docs/SignupSheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
-  <si>
-    <t>IP Address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
   <si>
     <t>Device Type</t>
   </si>
@@ -34,9 +31,6 @@
     <t>Device Code</t>
   </si>
   <si>
-    <t>MAC Address</t>
-  </si>
-  <si>
     <t>house1</t>
   </si>
   <si>
@@ -83,60 +77,6 @@
   </si>
   <si>
     <t>doorbell</t>
-  </si>
-  <si>
-    <t>192.168.1.2</t>
-  </si>
-  <si>
-    <t>192.168.1.3</t>
-  </si>
-  <si>
-    <t>192.168.1.4</t>
-  </si>
-  <si>
-    <t>192.168.1.5</t>
-  </si>
-  <si>
-    <t>192.168.1.6</t>
-  </si>
-  <si>
-    <t>192.168.1.7</t>
-  </si>
-  <si>
-    <t>192.168.1.8</t>
-  </si>
-  <si>
-    <t>192.168.1.9</t>
-  </si>
-  <si>
-    <t>192.168.1.10</t>
-  </si>
-  <si>
-    <t>192.168.1.11</t>
-  </si>
-  <si>
-    <t>192.168.1.12</t>
-  </si>
-  <si>
-    <t>192.168.1.13</t>
-  </si>
-  <si>
-    <t>192.168.1.14</t>
-  </si>
-  <si>
-    <t>192.168.1.15</t>
-  </si>
-  <si>
-    <t>192.168.1.16</t>
-  </si>
-  <si>
-    <t>192.168.1.17</t>
-  </si>
-  <si>
-    <t>192.168.1.18</t>
-  </si>
-  <si>
-    <t>192.168.1.19</t>
   </si>
   <si>
     <t>externaldoor</t>
@@ -145,8 +85,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,13 +98,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -217,12 +150,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -284,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,9 +248,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,6 +283,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,14 +459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -540,279 +474,227 @@
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -821,12 +703,8 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -835,12 +713,8 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -849,12 +723,8 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -863,12 +733,8 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -877,12 +743,8 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -891,12 +753,8 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -905,10 +763,6 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>